<commit_message>
update all room, but not check
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95C3F62-9BAB-469A-AA90-3532D690EFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA113888-D8A9-424A-8260-9C37163CE2EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>room name</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>can't check the shortcut</t>
+  </si>
+  <si>
+    <t>need to check again</t>
+  </si>
+  <si>
+    <t>not be able to use new system</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -466,6 +472,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
@@ -752,7 +759,7 @@
   <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +767,8 @@
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="6" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -795,7 +803,9 @@
         <v>42</v>
       </c>
       <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="E2" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
       <c r="H2" s="18"/>
@@ -807,7 +817,7 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -831,7 +841,7 @@
       <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="22"/>
       <c r="E5" s="22"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -844,7 +854,7 @@
       <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -857,7 +867,7 @@
       <c r="C7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="22"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -868,8 +878,8 @@
         <v>12</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="19"/>
@@ -879,8 +889,8 @@
         <v>13</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="19"/>
@@ -890,8 +900,8 @@
         <v>14</v>
       </c>
       <c r="C10" s="22"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="19"/>
@@ -901,8 +911,8 @@
         <v>15</v>
       </c>
       <c r="C11" s="22"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="19"/>
@@ -912,7 +922,8 @@
         <v>16</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="19"/>
@@ -922,8 +933,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="22"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="19"/>
@@ -934,7 +947,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="19"/>
@@ -945,7 +958,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="19"/>
@@ -958,7 +971,7 @@
         <v>44</v>
       </c>
       <c r="D16" s="16"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="19"/>
@@ -969,7 +982,7 @@
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="19"/>
@@ -980,7 +993,7 @@
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="19"/>
@@ -991,7 +1004,7 @@
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="19"/>
@@ -1002,7 +1015,7 @@
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="19"/>
@@ -1013,7 +1026,7 @@
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="19"/>
@@ -1024,7 +1037,7 @@
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="19"/>
@@ -1035,7 +1048,7 @@
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="19"/>
@@ -1046,7 +1059,7 @@
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="19"/>
@@ -1057,7 +1070,7 @@
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="19"/>
@@ -1068,7 +1081,7 @@
       </c>
       <c r="C26" s="22"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="19"/>
@@ -1079,7 +1092,7 @@
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="16"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="19"/>
@@ -1090,7 +1103,7 @@
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="E28" s="25"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
@@ -1101,7 +1114,7 @@
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
@@ -1112,7 +1125,7 @@
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="1"/>
       <c r="H30" s="19"/>
     </row>
@@ -1122,7 +1135,7 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="19"/>
@@ -1133,7 +1146,7 @@
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="22"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="19"/>
@@ -1144,7 +1157,7 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="19"/>
@@ -1155,7 +1168,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="19"/>
@@ -1166,7 +1179,7 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="19"/>
@@ -1177,7 +1190,7 @@
       </c>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
+      <c r="E36" s="25"/>
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
       <c r="H36" s="21"/>
@@ -1188,7 +1201,7 @@
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="E37" s="27"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>

</xml_diff>

<commit_message>
check almost all the room graphics
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA113888-D8A9-424A-8260-9C37163CE2EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1740C1-72C5-42FC-9E16-C475EAB3515F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>room name</t>
   </si>
@@ -166,13 +166,16 @@
   </si>
   <si>
     <t>not be able to use new system</t>
+  </si>
+  <si>
+    <t>need the view on the other room</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,20 +192,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,11 +208,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -432,13 +423,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -447,36 +437,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutre" xfId="3" builtinId="28"/>
+  <cellStyles count="3">
+    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -759,14 +747,14 @@
   <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
@@ -802,13 +790,13 @@
       <c r="C2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
@@ -817,11 +805,11 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="19"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
@@ -832,7 +820,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="19"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -841,11 +829,11 @@
       <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="19"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
@@ -854,11 +842,11 @@
       <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="19"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
@@ -867,267 +855,269 @@
       <c r="C7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="19"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="19"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="19"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="19"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="19"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="22"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="19"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="24"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="19"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="22"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="19"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="22"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="19"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="22"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="19"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="22"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="19"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="22"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="19"/>
+      <c r="H19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="22"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="19"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="22"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="19"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="22"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="19"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="22"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="19"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="22"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="19"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="22"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="19"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="22"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="21"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="19"/>
+      <c r="H26" s="18"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="22"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="19"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="21"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="18"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="22"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="22"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="1"/>
-      <c r="H30" s="19"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="12" t="s">
@@ -1135,43 +1125,43 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="22"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="19"/>
+      <c r="H31" s="18"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="22"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="19"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="22"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="19"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="22"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="19"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="s">
@@ -1179,21 +1169,21 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="22"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="19"/>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="21"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14" t="s">
@@ -1201,7 +1191,7 @@
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="27"/>
+      <c r="E37" s="26"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>

</xml_diff>

<commit_message>
add all the room that are in game on the map
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1740C1-72C5-42FC-9E16-C475EAB3515F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3BF6FC-1C84-4786-9D5A-11291E861EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +794,7 @@
       <c r="E2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="16"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="16"/>
       <c r="H2" s="17"/>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="1"/>
       <c r="H3" s="18"/>
     </row>
@@ -818,7 +818,7 @@
       <c r="C4" s="15"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="1"/>
       <c r="H4" s="18"/>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="1"/>
       <c r="H5" s="18"/>
     </row>
@@ -844,7 +844,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="1"/>
       <c r="H6" s="18"/>
     </row>
@@ -857,7 +857,7 @@
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="1"/>
       <c r="H7" s="18"/>
     </row>
@@ -868,7 +868,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="1"/>
       <c r="H8" s="18"/>
     </row>
@@ -879,7 +879,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="1"/>
       <c r="H9" s="18"/>
     </row>
@@ -890,7 +890,7 @@
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="1"/>
       <c r="H10" s="18"/>
     </row>
@@ -901,7 +901,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="1"/>
       <c r="H11" s="18"/>
     </row>
@@ -912,7 +912,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="23"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="1"/>
       <c r="H12" s="18"/>
     </row>
@@ -925,7 +925,7 @@
         <v>45</v>
       </c>
       <c r="E13" s="21"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="1"/>
       <c r="H13" s="18"/>
     </row>
@@ -936,7 +936,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="21"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="1"/>
       <c r="H14" s="18"/>
     </row>
@@ -947,7 +947,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="1"/>
       <c r="H15" s="18"/>
     </row>
@@ -960,7 +960,7 @@
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="1"/>
       <c r="H16" s="18"/>
     </row>
@@ -971,7 +971,7 @@
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="1"/>
       <c r="H17" s="18"/>
     </row>
@@ -982,7 +982,7 @@
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="1"/>
       <c r="H18" s="18"/>
     </row>
@@ -993,7 +993,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="1"/>
       <c r="H19" s="18"/>
     </row>
@@ -1004,7 +1004,7 @@
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="1"/>
       <c r="H20" s="18"/>
     </row>
@@ -1015,7 +1015,7 @@
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="1"/>
       <c r="H21" s="18"/>
     </row>
@@ -1026,7 +1026,7 @@
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="1"/>
       <c r="H22" s="18"/>
     </row>
@@ -1037,7 +1037,7 @@
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="1"/>
       <c r="H23" s="18"/>
     </row>
@@ -1048,7 +1048,7 @@
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="21"/>
       <c r="G24" s="1"/>
       <c r="H24" s="18"/>
     </row>
@@ -1059,7 +1059,7 @@
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="1"/>
       <c r="H25" s="18"/>
     </row>
@@ -1072,7 +1072,7 @@
         <v>47</v>
       </c>
       <c r="E26" s="21"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="1"/>
       <c r="H26" s="18"/>
     </row>
@@ -1083,7 +1083,7 @@
       <c r="C27" s="23"/>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="1"/>
       <c r="H27" s="18"/>
     </row>
@@ -1094,7 +1094,7 @@
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="19"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
     </row>
@@ -1105,7 +1105,7 @@
       <c r="C29" s="25"/>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
-      <c r="F29" s="16"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="16"/>
       <c r="H29" s="17"/>
     </row>
@@ -1116,7 +1116,7 @@
       <c r="C30" s="21"/>
       <c r="D30" s="1"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="21"/>
       <c r="H30" s="18"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="21"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="1"/>
       <c r="H31" s="18"/>
     </row>
@@ -1137,7 +1137,7 @@
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="1"/>
       <c r="H32" s="18"/>
     </row>
@@ -1148,7 +1148,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
-      <c r="F33" s="1"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="1"/>
       <c r="H33" s="18"/>
     </row>
@@ -1159,7 +1159,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="1"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="1"/>
       <c r="H34" s="18"/>
     </row>
@@ -1170,7 +1170,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="21"/>
-      <c r="F35" s="1"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="1"/>
       <c r="H35" s="18"/>
     </row>
@@ -1181,7 +1181,7 @@
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
       <c r="E36" s="24"/>
-      <c r="F36" s="19"/>
+      <c r="F36" s="24"/>
       <c r="G36" s="19"/>
       <c r="H36" s="20"/>
     </row>
@@ -1192,7 +1192,7 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="26"/>
-      <c r="F37" s="4"/>
+      <c r="F37" s="26"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
     </row>

</xml_diff>

<commit_message>
check the respawn room, update it to the new system, andchange localisation of the hud
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3BF6FC-1C84-4786-9D5A-11291E861EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BD3BCE-1A2C-428F-AAF5-8D9FC5DF87CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>room name</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>need the view on the other room</t>
+  </si>
+  <si>
+    <t>not the loop room</t>
   </si>
 </sst>
 </file>
@@ -746,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,11 +818,13 @@
       <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="21"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add grass to all room and some new assets
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BD3BCE-1A2C-428F-AAF5-8D9FC5DF87CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A597E4B-B435-41C6-9030-6E076A0BF054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>room name</t>
   </si>
@@ -172,13 +172,16 @@
   </si>
   <si>
     <t>not the loop room</t>
+  </si>
+  <si>
+    <t>no grass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +203,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +246,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -426,12 +441,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -465,8 +481,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
     <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
@@ -750,7 +772,7 @@
   <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +820,9 @@
         <v>46</v>
       </c>
       <c r="F2" s="25"/>
-      <c r="G2" s="16"/>
+      <c r="G2" s="27" t="s">
+        <v>49</v>
+      </c>
       <c r="H2" s="17"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -811,7 +835,7 @@
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -837,7 +861,7 @@
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="18"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -850,7 +874,7 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="18"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -863,7 +887,7 @@
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -874,7 +898,7 @@
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -885,7 +909,7 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -896,7 +920,7 @@
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -907,7 +931,7 @@
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -918,7 +942,7 @@
       <c r="D12" s="23"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -931,7 +955,7 @@
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -942,7 +966,7 @@
       <c r="D14" s="21"/>
       <c r="E14" s="23"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="22"/>
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -953,7 +977,7 @@
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -966,7 +990,7 @@
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="18"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -977,7 +1001,7 @@
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -988,7 +1012,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -999,7 +1023,7 @@
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1010,7 +1034,7 @@
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1021,7 +1045,7 @@
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1032,7 +1056,7 @@
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="22"/>
       <c r="H22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1043,7 +1067,7 @@
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1054,7 +1078,7 @@
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="18"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1065,7 +1089,7 @@
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1078,7 +1102,7 @@
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1089,7 +1113,7 @@
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
-      <c r="G27" s="1"/>
+      <c r="G27" s="22"/>
       <c r="H27" s="18"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1100,7 +1124,7 @@
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
-      <c r="G28" s="19"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="20"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1111,7 +1135,7 @@
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
-      <c r="G29" s="16"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1122,6 +1146,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
+      <c r="G30" s="30"/>
       <c r="H30" s="18"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1132,7 +1157,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
-      <c r="G31" s="1"/>
+      <c r="G31" s="22"/>
       <c r="H31" s="18"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1143,7 +1168,7 @@
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
-      <c r="G32" s="1"/>
+      <c r="G32" s="22"/>
       <c r="H32" s="18"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -1154,7 +1179,7 @@
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="22"/>
       <c r="H33" s="18"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -1165,7 +1190,7 @@
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
-      <c r="G34" s="1"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1176,7 +1201,7 @@
       <c r="D35" s="1"/>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
-      <c r="G35" s="1"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="18"/>
     </row>
     <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1187,7 +1212,7 @@
       <c r="D36" s="19"/>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
-      <c r="G36" s="19"/>
+      <c r="G36" s="28"/>
       <c r="H36" s="20"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1198,7 +1223,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="26"/>
       <c r="F37" s="26"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="31"/>
       <c r="H37" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change dza to add the door for dz and add rPla_c
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A597E4B-B435-41C6-9030-6E076A0BF054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943CF974-576A-42B7-A77B-27B334E2830B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>room name</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>no grass</t>
+  </si>
+  <si>
+    <t>rPla_c</t>
   </si>
 </sst>
 </file>
@@ -252,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -435,6 +438,45 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -447,7 +489,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -466,7 +508,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -480,12 +521,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
@@ -769,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H37"/>
+  <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,15 +859,15 @@
       <c r="C2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="27" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
@@ -832,24 +876,24 @@
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="18"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="18"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -858,11 +902,11 @@
       <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="18"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
@@ -871,11 +915,11 @@
       <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="18"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
@@ -884,270 +928,270 @@
       <c r="C7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="18"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="18"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="18"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="18"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="18"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="18"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="18"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="18"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="18"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="17"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="18"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="17"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="18"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="18"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="18"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="18"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="17"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22" t="s">
+      <c r="C26" s="20"/>
+      <c r="D26" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="18"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="18"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="17"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="20"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="19"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="17"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="21"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="18"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="12" t="s">
@@ -1155,43 +1199,43 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="18"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="17"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="18"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="17"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="18"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="17"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="18"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="17"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="s">
@@ -1199,32 +1243,43 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="18"/>
-    </row>
-    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="13" t="s">
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="17"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="20"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="19"/>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="5"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
count number of enemies in each room on the exel
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943CF974-576A-42B7-A77B-27B334E2830B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFC64B3-C865-4994-8660-8E97511AAE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>room name</t>
   </si>
@@ -178,13 +178,49 @@
   </si>
   <si>
     <t>rPla_c</t>
+  </si>
+  <si>
+    <t>number of enemies</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>need to add the view on the other zone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +245,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -444,13 +493,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -460,11 +509,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -473,10 +522,23 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -489,7 +551,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -497,7 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -512,24 +573,47 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
@@ -813,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H38"/>
+  <dimension ref="B1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,9 +911,11 @@
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -848,440 +934,557 @@
       <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="I1" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="D12" s="28"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="17"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="17"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="17"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21" t="s">
+      <c r="C26" s="16"/>
+      <c r="D26" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="17"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="17"/>
-    </row>
-    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10" t="s">
+      <c r="C27" s="28"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="19"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="16"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="17"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="17"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="12" t="s">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="17"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="17"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="12" t="s">
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="17"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="17"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="17"/>
-    </row>
-    <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="13" t="s">
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="19"/>
-    </row>
-    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="32" t="s">
+      <c r="G37" s="21"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="31"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="32">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat. forest tiles, door and key. rFor_a. fix rPla_jelly
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFC64B3-C865-4994-8660-8E97511AAE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D9433E-DBD5-41F2-80E0-FF404EC7261F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>room name</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>need to add the view on the other zone</t>
+  </si>
+  <si>
+    <t>boss</t>
+  </si>
+  <si>
+    <t>rPla_jelly</t>
+  </si>
+  <si>
+    <t>rFor_a</t>
   </si>
 </sst>
 </file>
@@ -263,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,8 +312,14 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -542,6 +557,17 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -551,7 +577,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -614,6 +640,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
@@ -897,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I38"/>
+  <dimension ref="B1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,6 +1512,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="42"/>
+      <c r="I39" s="37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="41" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat. all the room transition for the beta. Need to fix the dz problem
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D9433E-DBD5-41F2-80E0-FF404EC7261F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF292067-2997-44C0-9825-A21A73C55E43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="495" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>room name</t>
   </si>
@@ -223,6 +223,27 @@
   </si>
   <si>
     <t>rFor_a</t>
+  </si>
+  <si>
+    <t>rFor_a1</t>
+  </si>
+  <si>
+    <t>rFor_b1</t>
+  </si>
+  <si>
+    <t>AFTER WALL JUMP</t>
+  </si>
+  <si>
+    <t>rPla_key1</t>
+  </si>
+  <si>
+    <t>but the next dz room does not exist for the beta</t>
+  </si>
+  <si>
+    <t>but the next for room does not exist for the beta</t>
+  </si>
+  <si>
+    <t>but the next factory room does not exist for the beta</t>
   </si>
 </sst>
 </file>
@@ -272,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,8 +339,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -352,7 +379,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -367,7 +394,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -382,7 +409,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -394,7 +421,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -406,13 +433,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -421,13 +463,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -439,57 +496,34 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -499,74 +533,9 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -577,72 +546,63 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
@@ -926,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I40"/>
+  <dimension ref="B1:K118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,590 +901,1399 @@
     <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
     <col min="8" max="8" width="44.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="37" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="24" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="33">
+      <c r="H2" s="9"/>
+      <c r="I2" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="34">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="34">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="38">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="34">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="34" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="35">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="34">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="34">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="34">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="16">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="34">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="34">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="34">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="34">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="34">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="34">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="35">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="34" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="34">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="34">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="16">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="34">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="34">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="34">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="34">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="17" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="26" t="s">
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="34">
+      <c r="I26" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="34">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="9" t="s">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="39">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="33">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="34">
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="34">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="34">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="34">
+      <c r="C33" s="12"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="34">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="34">
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="34">
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="16">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="12" t="s">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="36">
+      <c r="C37" s="12"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="29" t="s">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="32">
+      <c r="C38" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="40" t="s">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="42"/>
-      <c r="I39" s="37" t="s">
+      <c r="C39" s="12"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="41" t="s">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="26" t="s">
         <v>57</v>
       </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="27"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="27"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="27"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="16"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="27"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="16"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="27"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="16"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="27"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="16"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="27"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="16"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="27"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="16"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="27"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="16"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="27"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="16"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="27"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="16"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="27"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="16"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="27"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="16"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="27"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="16"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="27"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="16"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="27"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="16"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="27"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="16"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="27"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="16"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="27"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="16"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="27"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="16"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="27"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="16"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="27"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="16"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="27"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="16"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="27"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="16"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="27"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="16"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="27"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="16"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="27"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="16"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="27"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="16"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="27"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="16"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="27"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="16"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="27"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="16"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="27"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="16"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="27"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="16"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="27"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="16"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="27"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="16"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="27"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="16"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="27"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="16"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="27"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="16"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="27"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="16"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="27"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="16"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="27"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="16"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="27"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="16"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="27"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="16"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="27"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="16"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="27"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="16"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="27"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="16"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="27"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="16"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="27"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="16"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="27"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="16"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="27"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="16"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="27"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="16"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="27"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="16"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="27"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="16"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="27"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="16"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="27"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="16"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="27"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="16"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="27"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="16"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="27"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="16"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="27"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="16"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="27"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="16"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="27"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="16"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="27"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="16"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="27"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="16"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="27"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="16"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="27"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="16"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="27"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="16"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="27"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="16"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="27"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="16"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="27"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="16"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="27"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="16"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="27"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="16"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="27"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="16"/>
+    </row>
+    <row r="118" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="28"/>
+      <c r="C118" s="10"/>
+      <c r="D118" s="10"/>
+      <c r="E118" s="10"/>
+      <c r="F118" s="10"/>
+      <c r="G118" s="10"/>
+      <c r="H118" s="10"/>
+      <c r="I118" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
clean. table of room
</commit_message>
<xml_diff>
--- a/room verification.xlsx
+++ b/room verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\_Social-ladder\social_ladder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF292067-2997-44C0-9825-A21A73C55E43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6E8EFA-0001-4517-A87D-58639E8C95E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="495" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +345,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -546,7 +552,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -603,6 +609,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="3" builtinId="27"/>
@@ -888,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1399,7 @@
       <c r="B33" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
@@ -1434,7 +1441,7 @@
       <c r="B36" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="34" t="s">
         <v>64</v>
       </c>
       <c r="D36" s="1"/>
@@ -1480,7 +1487,7 @@
       <c r="B39" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="12"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="1"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
@@ -1494,7 +1501,7 @@
       <c r="B40" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="12"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="1"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -1508,7 +1515,7 @@
       <c r="B41" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="1"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
@@ -1522,7 +1529,7 @@
       <c r="B42" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="1"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>

</xml_diff>